<commit_message>
chore: backup before Wisdom V2 refactoring
</commit_message>
<xml_diff>
--- a/.agent/スキル一覧.xlsx
+++ b/.agent/スキル一覧.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fate_\OneDrive\デスクトップ\OWLight_ZERO\owlight-mvp\.agent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fate_\OneDrive\デスクトップ\OWLight_ONE\.agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3ED216-095B-48A6-83C2-440FFDFD2B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5C7CC5-8553-4657-8901-11FAE64E6122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'新規 テキスト ドキュメント'!$A$1:$G$68</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'新規 テキスト ドキュメント'!$A$1:$G$70</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="251">
   <si>
     <t>スキルID</t>
   </si>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>GCS同期スクリプト</t>
-  </si>
-  <si>
-    <t>SupabaseのナレッジをJSONL形式でGCSバケットにアップロードするバッチ処理。</t>
   </si>
   <si>
     <t>infra-doc-extraction</t>
@@ -782,6 +779,48 @@
     <rPh sb="0" eb="2">
       <t>ケイカク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>validation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>infra-supabase-self-healing</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Supabase自己修復機能</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>接続障害検知、自動再接続、サーキットブレーカーを含む高可用性クライアントを実装する。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SupabaseのナレッジをJSONL形式でGCSバケットにアップロードするバッチ処理。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>integration</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>knowledge-ui-detail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ナレッジコラボレーション＆詳細画面</t>
+    <rPh sb="13" eb="15">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ガメン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リッチでコラボレーティブなナレッジ詳細画面 (V2) を実装するためのパターン定義。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -884,7 +923,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A869E180-AB61-428A-B49B-95B7424B86BA}" name="新規_テキスト_ドキュメント" displayName="新規_テキスト_ドキュメント" ref="A1:G68" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A869E180-AB61-428A-B49B-95B7424B86BA}" name="新規_テキスト_ドキュメント" displayName="新規_テキスト_ドキュメント" ref="A1:G70" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{EBA6607A-40C2-4282-9041-D5CD47B6C2B8}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{1B4C999D-2617-4CD9-8C9F-A079276CEFD8}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
@@ -1161,13 +1200,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A2B7BC-21A8-4B0C-BE59-F870DDB5A5C1}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -1183,10 +1222,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1465,20 +1504,18 @@
         <v>127</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" t="s">
-        <v>142</v>
+        <v>248</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
       </c>
-      <c r="G13" t="s">
-        <v>134</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -1488,13 +1525,13 @@
         <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -1505,25 +1542,25 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C15" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1534,19 +1571,19 @@
         <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1557,19 +1594,19 @@
         <v>147</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1580,13 +1617,13 @@
         <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
@@ -1603,19 +1640,19 @@
         <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>159</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1626,82 +1663,82 @@
         <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>220</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" t="s">
         <v>220</v>
       </c>
-      <c r="B22" t="s">
-        <v>221</v>
-      </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
         <v>220</v>
       </c>
-      <c r="B23" t="s">
-        <v>221</v>
-      </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
@@ -1712,42 +1749,42 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" t="s">
         <v>220</v>
       </c>
-      <c r="B24" t="s">
-        <v>221</v>
-      </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
         <v>220</v>
       </c>
-      <c r="B25" t="s">
-        <v>221</v>
-      </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
@@ -1758,88 +1795,88 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s">
         <v>222</v>
       </c>
-      <c r="B27" t="s">
-        <v>223</v>
-      </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" t="s">
         <v>222</v>
       </c>
-      <c r="B28" t="s">
-        <v>223</v>
-      </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" t="s">
         <v>222</v>
       </c>
-      <c r="B29" t="s">
-        <v>223</v>
-      </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F29" t="s">
         <v>18</v>
@@ -1850,157 +1887,157 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B31" t="s">
         <v>224</v>
       </c>
-      <c r="B31" t="s">
-        <v>225</v>
-      </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" t="s">
         <v>224</v>
       </c>
-      <c r="B32" t="s">
-        <v>225</v>
-      </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>223</v>
+      </c>
+      <c r="B33" t="s">
         <v>224</v>
       </c>
-      <c r="B33" t="s">
-        <v>225</v>
-      </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" t="s">
         <v>224</v>
       </c>
-      <c r="B34" t="s">
-        <v>225</v>
-      </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
+        <v>223</v>
+      </c>
+      <c r="B35" t="s">
         <v>224</v>
       </c>
-      <c r="B35" t="s">
-        <v>225</v>
-      </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" t="s">
         <v>224</v>
       </c>
-      <c r="B36" t="s">
-        <v>225</v>
-      </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F36" t="s">
         <v>18</v>
@@ -2011,25 +2048,25 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>177</v>
+        <v>223</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>226</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G37" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2040,19 +2077,19 @@
         <v>178</v>
       </c>
       <c r="C38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E38" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>179</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -2063,19 +2100,19 @@
         <v>178</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -2086,13 +2123,13 @@
         <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F40" t="s">
         <v>18</v>
@@ -2109,42 +2146,42 @@
         <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="E41" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="F41" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="F42" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2155,19 +2192,19 @@
         <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G43" t="s">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -2178,19 +2215,19 @@
         <v>161</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F44" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2201,19 +2238,19 @@
         <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E45" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G45" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -2224,62 +2261,62 @@
         <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F46" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G46" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>227</v>
+        <v>160</v>
       </c>
       <c r="B47" t="s">
         <v>161</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>57</v>
+        <v>176</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B48" t="s">
         <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G48" t="s">
         <v>7</v>
@@ -2287,48 +2324,48 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B49" t="s">
         <v>161</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F49" t="s">
         <v>18</v>
       </c>
       <c r="G49" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="B50" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>192</v>
+        <v>61</v>
       </c>
       <c r="D50" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
       <c r="E50" t="s">
-        <v>194</v>
+        <v>63</v>
       </c>
       <c r="F50" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G50" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2339,19 +2376,19 @@
         <v>191</v>
       </c>
       <c r="C51" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E51" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>192</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -2362,85 +2399,85 @@
         <v>191</v>
       </c>
       <c r="C52" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D52" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E52" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F52" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="B53" t="s">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>199</v>
       </c>
       <c r="E53" t="s">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="F53" t="s">
         <v>18</v>
       </c>
       <c r="G53" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
+        <v>227</v>
+      </c>
+      <c r="B54" t="s">
         <v>228</v>
       </c>
-      <c r="B54" t="s">
-        <v>229</v>
-      </c>
       <c r="C54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E54" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
         <v>18</v>
       </c>
       <c r="G54" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="B55" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="C55" t="s">
-        <v>203</v>
+        <v>92</v>
       </c>
       <c r="D55" t="s">
-        <v>204</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>205</v>
+        <v>94</v>
       </c>
       <c r="F55" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G55" t="s">
         <v>7</v>
@@ -2454,19 +2491,19 @@
         <v>202</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="D56" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F56" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>203</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2477,19 +2514,19 @@
         <v>202</v>
       </c>
       <c r="C57" t="s">
-        <v>208</v>
+        <v>70</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E57" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2500,19 +2537,19 @@
         <v>202</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
       <c r="D58" t="s">
-        <v>65</v>
+        <v>209</v>
       </c>
       <c r="E58" t="s">
-        <v>66</v>
+        <v>210</v>
       </c>
       <c r="F58" t="s">
         <v>18</v>
       </c>
       <c r="G58" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2523,19 +2560,19 @@
         <v>202</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F59" t="s">
         <v>18</v>
       </c>
       <c r="G59" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2546,42 +2583,42 @@
         <v>202</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D60" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F60" t="s">
         <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B61" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C61" t="s">
-        <v>213</v>
+        <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="E61" t="s">
-        <v>215</v>
+        <v>73</v>
       </c>
       <c r="F61" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="G61" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2592,19 +2629,19 @@
         <v>212</v>
       </c>
       <c r="C62" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D62" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E62" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="F62" t="s">
         <v>88</v>
       </c>
       <c r="G62" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2615,131 +2652,172 @@
         <v>212</v>
       </c>
       <c r="C63" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="D63" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="E63" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F63" t="s">
         <v>88</v>
       </c>
       <c r="G63" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="B64" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>243</v>
       </c>
       <c r="D64" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="E64" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="F64" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" t="s">
-        <v>7</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="B65" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="D65" t="s">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>231</v>
       </c>
       <c r="F65" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G65" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="B66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D66" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E66" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F66" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="G66" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" t="s">
+        <v>232</v>
+      </c>
+      <c r="C67" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
+        <v>101</v>
+      </c>
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" t="s">
+        <v>106</v>
+      </c>
+      <c r="E68" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" t="s">
+        <v>101</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>240</v>
+      </c>
+      <c r="B69" t="s">
         <v>241</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="C69" t="s">
+        <v>233</v>
+      </c>
+      <c r="D69" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" t="s">
+        <v>235</v>
+      </c>
+      <c r="F69" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>240</v>
+      </c>
+      <c r="B70" t="s">
+        <v>241</v>
+      </c>
+      <c r="C70" t="s">
+        <v>238</v>
+      </c>
+      <c r="D70" t="s">
+        <v>239</v>
+      </c>
+      <c r="E70" t="s">
         <v>237</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D68" s="1" t="s">
+      <c r="F70" t="s">
         <v>240</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="G68" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>